<commit_message>
evidence separation for batch and individual added
</commit_message>
<xml_diff>
--- a/Results/gpt-3.5-turbo-1106back_reasoningabd.xlsx
+++ b/Results/gpt-3.5-turbo-1106back_reasoningabd.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>ques_id</t>
   </si>
@@ -76,22 +76,19 @@
     <t>No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.</t>
   </si>
   <si>
-    <t>Leonardo DiCaprio does not have any children, so he does not have a third child.</t>
-  </si>
-  <si>
-    <t>The conclusion is not accurate.</t>
-  </si>
-  <si>
-    <t>The conclusion is plausible because the actor Leonardo DiCaprio does not have any children.</t>
-  </si>
-  <si>
-    <t>While it may be technically true that humans are animals and that Neil Armstrong was the first person to land on the moon, it is not accurate to consider him the first "animal" on the moon. This would be a misleading interpretation of the term "animal" in the context of space exploration. The statement fails to align with our broader understanding of sending animals to space and implicitly misleads the reader. Therefore, the conclusion is not accurate.</t>
-  </si>
-  <si>
-    <t>This conclusion aligns with the established fact that Leonardo DiCaprio has never been married and has no children, as corroborated by multiple credible sources. Therefore, the inference that he does not have a third child is logically sound and consistent with the information provided.</t>
-  </si>
-  <si>
-    <t>What was the species of the first living being to land on the Moon?</t>
+    <t>The conclusion is plausible because humans are technically animals, and thus, Neil Armstrong, as a human, could be considered the first animal sent to the Moon based on the premise.</t>
+  </si>
+  <si>
+    <t>It is highly plausible that Leonardo DiCaprio does not have any children.</t>
+  </si>
+  <si>
+    <t>The conclusion that humans, being animals, could be considered the first animal sent to the Moon, is plausible. This is because the premise states that no animals were ever sent to the Moon, and it is a fact that humans belong to the species Homo sapiens. Therefore, the conclusion logically follows from the given premise and aligns with our broader understanding of the classification of humans within the animal kingdom.</t>
+  </si>
+  <si>
+    <t>Leonardo DiCaprio has never been married, and there is no publicly available information or evidence to suggest that he has children. The lack of any reports, public acknowledgment, or visible presence of children strongly suggests that the conclusion about him not having any children is credible. This aligns with his public persona and is supported both by specific pieces of evidence and general knowledge about his personal life.</t>
+  </si>
+  <si>
+    <t>Who was technically the first animal sent to the Moon according to the given information?</t>
   </si>
   <si>
     <t>Does Leonardo DiCaprio have any children?</t>
@@ -100,7 +97,7 @@
     <t>{'Answer:': 'No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.', 'Source:': 'Study.com (https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.)', 'Premise of the Question:': 'Valid', 'Explanation:': ''}</t>
   </si>
   <si>
-    <t>{'Answer:': 'Leonardo DiCaprio does not have any children, so he does not have a third child.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have)', 'Premise of the Question:': 'Invalid', 'Explanation:': ''}</t>
+    <t>{'Answer:': 'Leonardo DiCaprio does not have any children.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have)', 'Premise of the Question:': 'InvalidLeonardo DiCaprio does not have any children, so the question contains a false premise.', 'Explanation:': ''}</t>
   </si>
   <si>
     <t>before 2022</t>
@@ -531,28 +528,28 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -566,31 +563,31 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic module import for fpdar added
</commit_message>
<xml_diff>
--- a/Results/gpt-3.5-turbo-1106back_reasoningabd.xlsx
+++ b/Results/gpt-3.5-turbo-1106back_reasoningabd.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>ques_id</t>
   </si>
@@ -76,19 +76,22 @@
     <t>No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.</t>
   </si>
   <si>
-    <t>The conclusion is plausible because humans are technically animals, and thus, Neil Armstrong, as a human, could be considered the first animal sent to the Moon based on the premise.</t>
-  </si>
-  <si>
-    <t>It is highly plausible that Leonardo DiCaprio does not have any children.</t>
-  </si>
-  <si>
-    <t>The conclusion that humans, being animals, could be considered the first animal sent to the Moon, is plausible. This is because the premise states that no animals were ever sent to the Moon, and it is a fact that humans belong to the species Homo sapiens. Therefore, the conclusion logically follows from the given premise and aligns with our broader understanding of the classification of humans within the animal kingdom.</t>
-  </si>
-  <si>
-    <t>Leonardo DiCaprio has never been married, and there is no publicly available information or evidence to suggest that he has children. The lack of any reports, public acknowledgment, or visible presence of children strongly suggests that the conclusion about him not having any children is credible. This aligns with his public persona and is supported both by specific pieces of evidence and general knowledge about his personal life.</t>
-  </si>
-  <si>
-    <t>Who was technically the first animal sent to the Moon according to the given information?</t>
+    <t>Leonardo DiCaprio does not have any children, so he does not have a third child.</t>
+  </si>
+  <si>
+    <t>The conclusion is not plausible.</t>
+  </si>
+  <si>
+    <t>The conclusion is highly plausible as Leonardo DiCaprio does not have any children.</t>
+  </si>
+  <si>
+    <t>The conclusion that Neil Armstrong was the first animal to land on the Moon is not plausible because humans are not typically referred to as animals in the context of space exploration. Additionally, historical records and scientific knowledge confirm that no animals were sent to the Moon, contradicting the conclusion drawn from the observation. Therefore, the conclusion is not logically and factually coherent with our understanding of reality.</t>
+  </si>
+  <si>
+    <t>Leonardo DiCaprio has never been married and has no children, as confirmed by reliable sources. Additionally, there is no credible information suggesting that he has any children. Therefore, the conclusion that he does not have a third child is highly credible and aligns with the available evidence and general knowledge.</t>
+  </si>
+  <si>
+    <t>Was Neil Armstrong the first animal to land on the moon?</t>
   </si>
   <si>
     <t>Does Leonardo DiCaprio have any children?</t>
@@ -97,7 +100,7 @@
     <t>{'Answer:': 'No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.', 'Source:': 'Study.com (https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.)', 'Premise of the Question:': 'Valid', 'Explanation:': ''}</t>
   </si>
   <si>
-    <t>{'Answer:': 'Leonardo DiCaprio does not have any children.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have)', 'Premise of the Question:': 'InvalidLeonardo DiCaprio does not have any children, so the question contains a false premise.', 'Explanation:': ''}</t>
+    <t>{'Answer:': 'Leonardo DiCaprio does not have any children, so he does not have a third child.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have)', 'Premise of the Question:': 'Invalid', 'Explanation:': ''}</t>
   </si>
   <si>
     <t>before 2022</t>
@@ -528,28 +531,28 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -563,31 +566,31 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>